<commit_message>
Added the window maximizing code line to all the pages. 4 tests are failing as there was a functionality change in the Login page. Should investigate further.
</commit_message>
<xml_diff>
--- a/src/main/java/resources/datasheets.xlsx
+++ b/src/main/java/resources/datasheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satya\Desktop\Eclipse Workspace\UITestingFramework-IntelliJ\src\main\java\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satya\eclipse-workspace\UITestingFramework-IntelliJ\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C6DF188-E023-4D09-9965-A876DC9B7C53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E044F-EFC8-4ADB-80B9-CD6257012DFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{FB8AC006-69BD-44BD-8808-042155A8488B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FB8AC006-69BD-44BD-8808-042155A8488B}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
@@ -443,16 +443,16 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,7 +480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -494,7 +494,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>